<commit_message>
doing this again :(
</commit_message>
<xml_diff>
--- a/cs2420/efficiency/mostly_sorted_data_comparisons_log.xlsx
+++ b/cs2420/efficiency/mostly_sorted_data_comparisons_log.xlsx
@@ -469,230 +469,350 @@
       <c r="A2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B2" t="n">
-        <v>5.614709844115208</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4.392317422778761</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4.087462841250339</v>
-      </c>
-      <c r="F2" t="n">
-        <v>4.321928094887363</v>
-      </c>
-      <c r="G2" t="n">
-        <v>3.807354922057604</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5.81</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4.39</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>4.09</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>4.46</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
-        <v>7.813781191217037</v>
-      </c>
-      <c r="C3" t="n">
-        <v>5.491853096329675</v>
-      </c>
-      <c r="D3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5.491853096329675</v>
-      </c>
-      <c r="F3" t="n">
-        <v>6.321928094887363</v>
-      </c>
-      <c r="G3" t="n">
-        <v>5.357552004618084</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>7.91</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5.49</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5.46</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>6.67</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>5.61</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B4" t="n">
-        <v>9.954196310386875</v>
-      </c>
-      <c r="C4" t="n">
-        <v>6.539158811108031</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6.768184324776926</v>
-      </c>
-      <c r="F4" t="n">
-        <v>8.312882955284355</v>
-      </c>
-      <c r="G4" t="n">
-        <v>6.78135971352466</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9.95</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>6.54</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>6.77</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>8.37</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6.79</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B5" t="n">
-        <v>11.95455984699983</v>
-      </c>
-      <c r="C5" t="n">
-        <v>7.562242424221073</v>
-      </c>
-      <c r="D5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E5" t="n">
-        <v>7.98299357469431</v>
-      </c>
-      <c r="F5" t="n">
-        <v>10.3297963382207</v>
-      </c>
-      <c r="G5" t="n">
-        <v>8.124121311829187</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.95</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>7.56</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>6.00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>7.98</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>10.30</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>8.08</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
-        <v>13.98868468677217</v>
-      </c>
-      <c r="C6" t="n">
-        <v>8.573647187493322</v>
-      </c>
-      <c r="D6" t="n">
-        <v>7</v>
-      </c>
-      <c r="E6" t="n">
-        <v>9.162391328756906</v>
-      </c>
-      <c r="F6" t="n">
-        <v>12.28511318850149</v>
-      </c>
-      <c r="G6" t="n">
-        <v>9.39231742277876</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>13.98</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>8.57</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>7.00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>9.16</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>12.21</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>9.41</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B7" t="n">
-        <v>15.99435343685886</v>
-      </c>
-      <c r="C7" t="n">
-        <v>9.579315937580015</v>
-      </c>
-      <c r="D7" t="n">
-        <v>8</v>
-      </c>
-      <c r="E7" t="n">
-        <v>10.31854280970272</v>
-      </c>
-      <c r="F7" t="n">
-        <v>14.41303285326386</v>
-      </c>
-      <c r="G7" t="n">
-        <v>10.63843591399047</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>15.99</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>9.58</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>8.00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>10.32</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>14.40</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>10.63</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B8" t="n">
-        <v>17.99435896187524</v>
-      </c>
-      <c r="C8" t="n">
-        <v>10.58214198165878</v>
-      </c>
-      <c r="D8" t="n">
-        <v>9</v>
-      </c>
-      <c r="E8" t="n">
-        <v>11.4578938373147</v>
-      </c>
-      <c r="F8" t="n">
-        <v>16.35531668057918</v>
-      </c>
-      <c r="G8" t="n">
-        <v>11.852919585124</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>18.00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10.58</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>9.00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>11.46</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>16.33</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>11.86</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B9" t="n">
-        <v>19.99718085949066</v>
-      </c>
-      <c r="C9" t="n">
-        <v>11.58355293046649</v>
-      </c>
-      <c r="D9" t="n">
-        <v>10</v>
-      </c>
-      <c r="E9" t="n">
-        <v>12.58378795450234</v>
-      </c>
-      <c r="F9" t="n">
-        <v>18.32700872412068</v>
-      </c>
-      <c r="G9" t="n">
-        <v>13.04046097095658</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>11.58</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>12.58</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>18.34</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>13.04</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B10" t="n">
-        <v>21.99929538702341</v>
-      </c>
-      <c r="C10" t="n">
-        <v>12.58425788774457</v>
-      </c>
-      <c r="D10" t="n">
-        <v>11</v>
-      </c>
-      <c r="E10" t="n">
-        <v>13.70011455491349</v>
-      </c>
-      <c r="F10" t="n">
-        <v>20.35105892074899</v>
-      </c>
-      <c r="G10" t="n">
-        <v>14.20319503738126</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>22.00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12.58</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>11.00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>13.70</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>20.34</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>14.20</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B11" t="n">
-        <v>23.99964773652837</v>
-      </c>
-      <c r="C11" t="n">
-        <v>13.58461023724953</v>
-      </c>
-      <c r="D11" t="n">
-        <v>12</v>
-      </c>
-      <c r="E11" t="n">
-        <v>14.80720396253033</v>
-      </c>
-      <c r="F11" t="n">
-        <v>22.3174164782476</v>
-      </c>
-      <c r="G11" t="n">
-        <v>15.35187094333514</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>24.00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>13.58</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>12.00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>14.81</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>22.33</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>15.35</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>